<commit_message>
superman sound is STEREO
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15070" uniqueCount="5196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15071" uniqueCount="5197">
   <si>
     <t>pacman</t>
   </si>
@@ -15643,6 +15643,9 @@
   </si>
   <si>
     <t>rastan sndhrdw</t>
+  </si>
+  <si>
+    <t>STEREO SOUND</t>
   </si>
 </sst>
 </file>
@@ -15966,10 +15969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15981,9 +15984,10 @@
     <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1638</v>
       </c>
@@ -16008,8 +16012,11 @@
       <c r="Q1" t="s">
         <v>5195</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>5196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3121</v>
       </c>
@@ -16035,7 +16042,7 @@
         <v>3123</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3124</v>
       </c>
@@ -16061,7 +16068,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4170</v>
       </c>
@@ -16084,7 +16091,7 @@
         <v>4172</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4173</v>
       </c>
@@ -16107,7 +16114,7 @@
         <v>4174</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4175</v>
       </c>
@@ -16133,7 +16140,7 @@
         <v>4176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4177</v>
       </c>

</xml_diff>